<commit_message>
found mistake in data (field.ID); create Gather scripts for two more datasets (2nd/3rd order data; Create Barplots with error bars;
</commit_message>
<xml_diff>
--- a/Data/F2_EW_Data.xlsx
+++ b/Data/F2_EW_Data.xlsx
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BG11" sqref="BG11"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -19214,7 +19214,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>84</v>
@@ -83930,7 +83930,7 @@
       </c>
       <c r="B90">
         <f>F1_EW_Total!B90</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C90">
         <f>F1_EW_Total!S90</f>

</xml_diff>